<commit_message>
shashank_parth_rohan Accounting for null values
</commit_message>
<xml_diff>
--- a/Ssl/Splitwise/Transactions_rohan.xlsx
+++ b/Ssl/Splitwise/Transactions_rohan.xlsx
@@ -363,8 +363,8 @@
     <col customWidth="1" max="2" min="2" width="20"/>
     <col customWidth="1" max="3" min="3" width="20"/>
     <col customWidth="1" max="4" min="4" width="20"/>
-    <col customWidth="1" max="5" min="5" width="30"/>
-    <col customWidth="1" max="6" min="6" width="20"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
+    <col customWidth="1" max="6" min="6" width="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -380,20 +380,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Type of Expense</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Date and Time of Transaction</t>
         </is>
       </c>
-      <c r="F1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -408,15 +412,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>ssl2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>78.00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Movies</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>2019-11-25 00:40:48.856459</t>
         </is>
@@ -435,15 +444,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>ssl2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>78.00</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Movies</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>2019-11-25 00:40:48.868418</t>
         </is>
@@ -462,15 +476,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>ssl2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>78.00</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Movies</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>2019-11-25 00:40:48.906311</t>
         </is>
@@ -489,15 +508,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>200.00</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Movies</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>2019-11-25 00:34:43.785197</t>
         </is>
@@ -516,15 +540,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>50.00</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Electronics</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>2019-11-25 00:35:16.699640</t>
         </is>
@@ -543,15 +572,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>250.00</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Food</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>2019-11-25 00:35:42.918846</t>
         </is>
@@ -570,15 +604,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>300.00</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Shopping</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>2019-11-25 00:39:03.766857</t>
         </is>
@@ -597,15 +636,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>che</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>75.00</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Travel</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>2019-11-25 00:39:47.480524</t>
         </is>
@@ -624,15 +668,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>ssl work</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>200.00</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Food</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>2019-11-25 00:40:19.242507</t>
         </is>
@@ -651,15 +700,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>ssl</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>200.00</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Electronics</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>2019-11-25 00:41:14.125654</t>
         </is>

</xml_diff>